<commit_message>
formatting added more comments to functions
</commit_message>
<xml_diff>
--- a/Sample/Conductor_Prop-Sample.xlsx
+++ b/Sample/Conductor_Prop-Sample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8784a4c37ac16e51/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8784a4c37ac16e51/Documents/Projects/Python/IEEE738-2012/Sample/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="8_{ECF437FA-FB1D-4E14-8876-DF79D5BCC045}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7ECBF004-8FF0-499D-8FDB-CC208FCE68A1}"/>
+  <xr:revisionPtr revIDLastSave="31" documentId="8_{ECF437FA-FB1D-4E14-8876-DF79D5BCC045}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{206A975D-DFD0-4E63-B707-CF369B23463E}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{6085CC8B-1036-44B9-9707-F15418EBC438}"/>
+    <workbookView xWindow="1140" yWindow="1140" windowWidth="28800" windowHeight="15370" xr2:uid="{6085CC8B-1036-44B9-9707-F15418EBC438}"/>
   </bookViews>
   <sheets>
     <sheet name="conductors" sheetId="1" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="76">
   <si>
     <t>Size</t>
   </si>
@@ -284,6 +284,12 @@
   </si>
   <si>
     <t>Core OD Units</t>
+  </si>
+  <si>
+    <t>PECO</t>
+  </si>
+  <si>
+    <t>`</t>
   </si>
 </sst>
 </file>
@@ -351,7 +357,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Data Input"/>
@@ -521,10 +527,6 @@
     </sheetDataSet>
   </externalBook>
 </externalLink>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -825,11 +827,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37CC4BCD-4400-4E7C-96DC-CDFA2CE28B1F}">
   <sheetPr codeName="Sheet22"/>
-  <dimension ref="A1:AB32"/>
+  <dimension ref="A1:AB33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B20" sqref="B20"/>
+      <selection pane="bottomLeft" activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -3747,6 +3749,9 @@
       <c r="Y24" s="1">
         <v>207.6</v>
       </c>
+      <c r="AA24" s="1" t="s">
+        <v>75</v>
+      </c>
       <c r="AB24" s="1" t="s">
         <v>12</v>
       </c>
@@ -4275,6 +4280,50 @@
       </c>
       <c r="AB32" s="1" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C33" s="1">
+        <v>555</v>
+      </c>
+      <c r="D33" s="1">
+        <v>55</v>
+      </c>
+      <c r="E33" s="1">
+        <v>4</v>
+      </c>
+      <c r="F33" s="1">
+        <v>0.16439999999999999</v>
+      </c>
+      <c r="L33" s="1">
+        <v>1.1508</v>
+      </c>
+      <c r="Q33" s="1">
+        <v>25</v>
+      </c>
+      <c r="R33" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="S33" s="1">
+        <v>75</v>
+      </c>
+      <c r="T33" s="1">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="U33" s="1">
+        <v>7.4399999999999994E-2</v>
+      </c>
+      <c r="V33" s="1">
+        <v>5280</v>
+      </c>
+      <c r="W33" s="1" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added demo file Moved methods from main.py to demo.py. cleaned up code added more comments added units for heat capacity
</commit_message>
<xml_diff>
--- a/Sample/Conductor_Prop-Sample.xlsx
+++ b/Sample/Conductor_Prop-Sample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8784a4c37ac16e51/Documents/Projects/Python/IEEE738-2012/Sample/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="31" documentId="8_{ECF437FA-FB1D-4E14-8876-DF79D5BCC045}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{206A975D-DFD0-4E63-B707-CF369B23463E}"/>
+  <xr:revisionPtr revIDLastSave="40" documentId="8_{ECF437FA-FB1D-4E14-8876-DF79D5BCC045}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ADFBADF2-4E57-4BF4-A0E0-9A51D3E0C84A}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="1140" windowWidth="28800" windowHeight="15370" xr2:uid="{6085CC8B-1036-44B9-9707-F15418EBC438}"/>
+    <workbookView xWindow="14230" yWindow="1000" windowWidth="10980" windowHeight="14240" xr2:uid="{6085CC8B-1036-44B9-9707-F15418EBC438}"/>
   </bookViews>
   <sheets>
     <sheet name="conductors" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <externalReference r:id="rId3"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">conductors!$A$1:$WWI$32</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">conductors!$A$1:$WWJ$32</definedName>
     <definedName name="absor">'[1]Data Input'!$E$13</definedName>
     <definedName name="angle">'[1]Data Input'!$I$33</definedName>
     <definedName name="atmosphere">'[1]Data Input'!$E$25</definedName>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="76">
   <si>
     <t>Size</t>
   </si>
@@ -286,10 +286,10 @@
     <t>Core OD Units</t>
   </si>
   <si>
-    <t>PECO</t>
-  </si>
-  <si>
-    <t>`</t>
+    <t>specific heat weight unit</t>
+  </si>
+  <si>
+    <t>J/(lb-C)</t>
   </si>
 </sst>
 </file>
@@ -307,12 +307,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -327,7 +333,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -338,6 +344,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -527,6 +536,10 @@
     </sheetDataSet>
   </externalBook>
 </externalLink>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -827,11 +840,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37CC4BCD-4400-4E7C-96DC-CDFA2CE28B1F}">
   <sheetPr codeName="Sheet22"/>
-  <dimension ref="A1:AB33"/>
+  <dimension ref="A1:AC32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D28" sqref="D28"/>
+      <selection pane="bottomLeft" activeCell="AA26" sqref="AA26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -863,1208 +876,1209 @@
     <col min="25" max="25" width="10.90625" style="1" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="12.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="12.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="263" width="11.453125" style="1"/>
-    <col min="264" max="264" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="265" max="265" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="266" max="266" width="11.453125" style="1"/>
-    <col min="267" max="267" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="268" max="268" width="10.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="269" max="269" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="270" max="270" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="271" max="271" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="272" max="272" width="8.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="273" max="273" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="274" max="274" width="8.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="275" max="275" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="276" max="276" width="9.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="277" max="279" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="280" max="280" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="281" max="281" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="282" max="282" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="283" max="283" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="284" max="519" width="11.453125" style="1"/>
-    <col min="520" max="520" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="521" max="521" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="522" max="522" width="11.453125" style="1"/>
-    <col min="523" max="523" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="524" max="524" width="10.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="525" max="525" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="526" max="526" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="527" max="527" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="528" max="528" width="8.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="529" max="529" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="530" max="530" width="8.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="531" max="531" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="532" max="532" width="9.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="533" max="535" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="536" max="536" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="537" max="537" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="538" max="538" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="539" max="539" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="540" max="775" width="11.453125" style="1"/>
-    <col min="776" max="776" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="777" max="777" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="778" max="778" width="11.453125" style="1"/>
-    <col min="779" max="779" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="780" max="780" width="10.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="781" max="781" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="782" max="782" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="783" max="783" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="784" max="784" width="8.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="785" max="785" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="786" max="786" width="8.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="787" max="787" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="788" max="788" width="9.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="789" max="791" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="792" max="792" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="793" max="793" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="794" max="794" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="795" max="795" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="796" max="1031" width="11.453125" style="1"/>
-    <col min="1032" max="1032" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="1033" max="1033" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="1034" max="1034" width="11.453125" style="1"/>
-    <col min="1035" max="1035" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="1036" max="1036" width="10.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="1037" max="1037" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="1038" max="1038" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="1039" max="1039" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="1040" max="1040" width="8.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="1041" max="1041" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="1042" max="1042" width="8.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="1043" max="1043" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="1044" max="1044" width="9.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="1045" max="1047" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="1048" max="1048" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="1049" max="1049" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="1050" max="1050" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="1051" max="1051" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="1052" max="1287" width="11.453125" style="1"/>
-    <col min="1288" max="1288" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="1289" max="1289" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="1290" max="1290" width="11.453125" style="1"/>
-    <col min="1291" max="1291" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="1292" max="1292" width="10.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="1293" max="1293" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="1294" max="1294" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="1295" max="1295" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="1296" max="1296" width="8.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="1297" max="1297" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="1298" max="1298" width="8.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="1299" max="1299" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="1300" max="1300" width="9.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="1301" max="1303" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="1304" max="1304" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="1305" max="1305" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="1306" max="1306" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="1307" max="1307" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="1308" max="1543" width="11.453125" style="1"/>
-    <col min="1544" max="1544" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="1545" max="1545" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="1546" max="1546" width="11.453125" style="1"/>
-    <col min="1547" max="1547" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="1548" max="1548" width="10.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="1549" max="1549" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="1550" max="1550" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="1551" max="1551" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="1552" max="1552" width="8.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="1553" max="1553" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="1554" max="1554" width="8.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="1555" max="1555" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="1556" max="1556" width="9.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="1557" max="1559" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="1560" max="1560" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="1561" max="1561" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="1562" max="1562" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="1563" max="1563" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="1564" max="1799" width="11.453125" style="1"/>
-    <col min="1800" max="1800" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="1801" max="1801" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="1802" max="1802" width="11.453125" style="1"/>
-    <col min="1803" max="1803" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="1804" max="1804" width="10.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="1805" max="1805" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="1806" max="1806" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="1807" max="1807" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="1808" max="1808" width="8.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="1809" max="1809" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="1810" max="1810" width="8.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="1811" max="1811" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="1812" max="1812" width="9.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="1813" max="1815" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="1816" max="1816" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="1817" max="1817" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="1818" max="1818" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="1819" max="1819" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="1820" max="2055" width="11.453125" style="1"/>
-    <col min="2056" max="2056" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2057" max="2057" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2058" max="2058" width="11.453125" style="1"/>
-    <col min="2059" max="2059" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2060" max="2060" width="10.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2061" max="2061" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2062" max="2062" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2063" max="2063" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2064" max="2064" width="8.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2065" max="2065" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="2066" max="2066" width="8.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2067" max="2067" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="2068" max="2068" width="9.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2069" max="2071" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2072" max="2072" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2073" max="2073" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2074" max="2074" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2075" max="2075" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2076" max="2311" width="11.453125" style="1"/>
-    <col min="2312" max="2312" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2313" max="2313" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2314" max="2314" width="11.453125" style="1"/>
-    <col min="2315" max="2315" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2316" max="2316" width="10.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2317" max="2317" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2318" max="2318" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2319" max="2319" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2320" max="2320" width="8.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2321" max="2321" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="2322" max="2322" width="8.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2323" max="2323" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="2324" max="2324" width="9.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2325" max="2327" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2328" max="2328" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2329" max="2329" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2330" max="2330" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2331" max="2331" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2332" max="2567" width="11.453125" style="1"/>
-    <col min="2568" max="2568" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2569" max="2569" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2570" max="2570" width="11.453125" style="1"/>
-    <col min="2571" max="2571" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2572" max="2572" width="10.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2573" max="2573" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2574" max="2574" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2575" max="2575" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2576" max="2576" width="8.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2577" max="2577" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="2578" max="2578" width="8.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2579" max="2579" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="2580" max="2580" width="9.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2581" max="2583" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2584" max="2584" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2585" max="2585" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2586" max="2586" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2587" max="2587" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2588" max="2823" width="11.453125" style="1"/>
-    <col min="2824" max="2824" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2825" max="2825" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2826" max="2826" width="11.453125" style="1"/>
-    <col min="2827" max="2827" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2828" max="2828" width="10.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2829" max="2829" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2830" max="2830" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2831" max="2831" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2832" max="2832" width="8.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2833" max="2833" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="2834" max="2834" width="8.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2835" max="2835" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="2836" max="2836" width="9.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2837" max="2839" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2840" max="2840" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2841" max="2841" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2842" max="2842" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2843" max="2843" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2844" max="3079" width="11.453125" style="1"/>
-    <col min="3080" max="3080" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3081" max="3081" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3082" max="3082" width="11.453125" style="1"/>
-    <col min="3083" max="3083" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3084" max="3084" width="10.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3085" max="3085" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3086" max="3086" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3087" max="3087" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3088" max="3088" width="8.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3089" max="3089" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="3090" max="3090" width="8.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3091" max="3091" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="3092" max="3092" width="9.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3093" max="3095" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3096" max="3096" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3097" max="3097" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3098" max="3098" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3099" max="3099" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3100" max="3335" width="11.453125" style="1"/>
-    <col min="3336" max="3336" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3337" max="3337" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3338" max="3338" width="11.453125" style="1"/>
-    <col min="3339" max="3339" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3340" max="3340" width="10.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3341" max="3341" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3342" max="3342" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3343" max="3343" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3344" max="3344" width="8.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3345" max="3345" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="3346" max="3346" width="8.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3347" max="3347" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="3348" max="3348" width="9.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3349" max="3351" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3352" max="3352" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3353" max="3353" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3354" max="3354" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3355" max="3355" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3356" max="3591" width="11.453125" style="1"/>
-    <col min="3592" max="3592" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3593" max="3593" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3594" max="3594" width="11.453125" style="1"/>
-    <col min="3595" max="3595" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3596" max="3596" width="10.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3597" max="3597" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3598" max="3598" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3599" max="3599" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3600" max="3600" width="8.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3601" max="3601" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="3602" max="3602" width="8.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3603" max="3603" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="3604" max="3604" width="9.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3605" max="3607" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3608" max="3608" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3609" max="3609" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3610" max="3610" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3611" max="3611" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3612" max="3847" width="11.453125" style="1"/>
-    <col min="3848" max="3848" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3849" max="3849" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3850" max="3850" width="11.453125" style="1"/>
-    <col min="3851" max="3851" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3852" max="3852" width="10.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3853" max="3853" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3854" max="3854" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3855" max="3855" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3856" max="3856" width="8.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3857" max="3857" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="3858" max="3858" width="8.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3859" max="3859" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="3860" max="3860" width="9.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3861" max="3863" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3864" max="3864" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3865" max="3865" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3866" max="3866" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3867" max="3867" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3868" max="4103" width="11.453125" style="1"/>
-    <col min="4104" max="4104" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4105" max="4105" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4106" max="4106" width="11.453125" style="1"/>
-    <col min="4107" max="4107" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4108" max="4108" width="10.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4109" max="4109" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4110" max="4110" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4111" max="4111" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4112" max="4112" width="8.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4113" max="4113" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="4114" max="4114" width="8.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4115" max="4115" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="4116" max="4116" width="9.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4117" max="4119" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4120" max="4120" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4121" max="4121" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4122" max="4122" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4123" max="4123" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4124" max="4359" width="11.453125" style="1"/>
-    <col min="4360" max="4360" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4361" max="4361" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4362" max="4362" width="11.453125" style="1"/>
-    <col min="4363" max="4363" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4364" max="4364" width="10.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4365" max="4365" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4366" max="4366" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4367" max="4367" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4368" max="4368" width="8.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4369" max="4369" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="4370" max="4370" width="8.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4371" max="4371" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="4372" max="4372" width="9.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4373" max="4375" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4376" max="4376" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4377" max="4377" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4378" max="4378" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4379" max="4379" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4380" max="4615" width="11.453125" style="1"/>
-    <col min="4616" max="4616" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4617" max="4617" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4618" max="4618" width="11.453125" style="1"/>
-    <col min="4619" max="4619" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4620" max="4620" width="10.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4621" max="4621" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4622" max="4622" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4623" max="4623" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4624" max="4624" width="8.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4625" max="4625" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="4626" max="4626" width="8.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4627" max="4627" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="4628" max="4628" width="9.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4629" max="4631" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4632" max="4632" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4633" max="4633" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4634" max="4634" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4635" max="4635" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4636" max="4871" width="11.453125" style="1"/>
-    <col min="4872" max="4872" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4873" max="4873" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4874" max="4874" width="11.453125" style="1"/>
-    <col min="4875" max="4875" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4876" max="4876" width="10.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4877" max="4877" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4878" max="4878" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4879" max="4879" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4880" max="4880" width="8.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4881" max="4881" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="4882" max="4882" width="8.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4883" max="4883" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="4884" max="4884" width="9.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4885" max="4887" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4888" max="4888" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4889" max="4889" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4890" max="4890" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4891" max="4891" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4892" max="5127" width="11.453125" style="1"/>
-    <col min="5128" max="5128" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5129" max="5129" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5130" max="5130" width="11.453125" style="1"/>
-    <col min="5131" max="5131" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5132" max="5132" width="10.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5133" max="5133" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5134" max="5134" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5135" max="5135" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5136" max="5136" width="8.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5137" max="5137" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="5138" max="5138" width="8.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5139" max="5139" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="5140" max="5140" width="9.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5141" max="5143" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5144" max="5144" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5145" max="5145" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5146" max="5146" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5147" max="5147" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5148" max="5383" width="11.453125" style="1"/>
-    <col min="5384" max="5384" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5385" max="5385" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5386" max="5386" width="11.453125" style="1"/>
-    <col min="5387" max="5387" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5388" max="5388" width="10.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5389" max="5389" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5390" max="5390" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5391" max="5391" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5392" max="5392" width="8.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5393" max="5393" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="5394" max="5394" width="8.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5395" max="5395" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="5396" max="5396" width="9.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5397" max="5399" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5400" max="5400" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5401" max="5401" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5402" max="5402" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5403" max="5403" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5404" max="5639" width="11.453125" style="1"/>
-    <col min="5640" max="5640" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5641" max="5641" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5642" max="5642" width="11.453125" style="1"/>
-    <col min="5643" max="5643" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5644" max="5644" width="10.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5645" max="5645" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5646" max="5646" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5647" max="5647" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5648" max="5648" width="8.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5649" max="5649" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="5650" max="5650" width="8.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5651" max="5651" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="5652" max="5652" width="9.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5653" max="5655" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5656" max="5656" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5657" max="5657" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5658" max="5658" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5659" max="5659" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5660" max="5895" width="11.453125" style="1"/>
-    <col min="5896" max="5896" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5897" max="5897" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5898" max="5898" width="11.453125" style="1"/>
-    <col min="5899" max="5899" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5900" max="5900" width="10.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5901" max="5901" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5902" max="5902" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5903" max="5903" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5904" max="5904" width="8.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5905" max="5905" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="5906" max="5906" width="8.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5907" max="5907" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="5908" max="5908" width="9.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5909" max="5911" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5912" max="5912" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5913" max="5913" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5914" max="5914" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5915" max="5915" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5916" max="6151" width="11.453125" style="1"/>
-    <col min="6152" max="6152" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6153" max="6153" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6154" max="6154" width="11.453125" style="1"/>
-    <col min="6155" max="6155" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6156" max="6156" width="10.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6157" max="6157" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6158" max="6158" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6159" max="6159" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6160" max="6160" width="8.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6161" max="6161" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="6162" max="6162" width="8.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6163" max="6163" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="6164" max="6164" width="9.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6165" max="6167" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6168" max="6168" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6169" max="6169" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6170" max="6170" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6171" max="6171" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6172" max="6407" width="11.453125" style="1"/>
-    <col min="6408" max="6408" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6409" max="6409" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6410" max="6410" width="11.453125" style="1"/>
-    <col min="6411" max="6411" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6412" max="6412" width="10.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6413" max="6413" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6414" max="6414" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6415" max="6415" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6416" max="6416" width="8.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6417" max="6417" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="6418" max="6418" width="8.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6419" max="6419" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="6420" max="6420" width="9.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6421" max="6423" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6424" max="6424" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6425" max="6425" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6426" max="6426" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6427" max="6427" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6428" max="6663" width="11.453125" style="1"/>
-    <col min="6664" max="6664" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6665" max="6665" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6666" max="6666" width="11.453125" style="1"/>
-    <col min="6667" max="6667" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6668" max="6668" width="10.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6669" max="6669" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6670" max="6670" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6671" max="6671" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6672" max="6672" width="8.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6673" max="6673" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="6674" max="6674" width="8.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6675" max="6675" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="6676" max="6676" width="9.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6677" max="6679" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6680" max="6680" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6681" max="6681" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6682" max="6682" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6683" max="6683" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6684" max="6919" width="11.453125" style="1"/>
-    <col min="6920" max="6920" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6921" max="6921" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6922" max="6922" width="11.453125" style="1"/>
-    <col min="6923" max="6923" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6924" max="6924" width="10.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6925" max="6925" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6926" max="6926" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6927" max="6927" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6928" max="6928" width="8.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6929" max="6929" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="6930" max="6930" width="8.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6931" max="6931" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="6932" max="6932" width="9.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6933" max="6935" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6936" max="6936" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6937" max="6937" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6938" max="6938" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6939" max="6939" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6940" max="7175" width="11.453125" style="1"/>
-    <col min="7176" max="7176" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7177" max="7177" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7178" max="7178" width="11.453125" style="1"/>
-    <col min="7179" max="7179" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7180" max="7180" width="10.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7181" max="7181" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7182" max="7182" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7183" max="7183" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7184" max="7184" width="8.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7185" max="7185" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="7186" max="7186" width="8.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7187" max="7187" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="7188" max="7188" width="9.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7189" max="7191" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7192" max="7192" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7193" max="7193" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7194" max="7194" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7195" max="7195" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7196" max="7431" width="11.453125" style="1"/>
-    <col min="7432" max="7432" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7433" max="7433" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7434" max="7434" width="11.453125" style="1"/>
-    <col min="7435" max="7435" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7436" max="7436" width="10.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7437" max="7437" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7438" max="7438" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7439" max="7439" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7440" max="7440" width="8.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7441" max="7441" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="7442" max="7442" width="8.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7443" max="7443" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="7444" max="7444" width="9.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7445" max="7447" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7448" max="7448" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7449" max="7449" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7450" max="7450" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7451" max="7451" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7452" max="7687" width="11.453125" style="1"/>
-    <col min="7688" max="7688" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7689" max="7689" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7690" max="7690" width="11.453125" style="1"/>
-    <col min="7691" max="7691" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7692" max="7692" width="10.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7693" max="7693" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7694" max="7694" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7695" max="7695" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7696" max="7696" width="8.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7697" max="7697" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="7698" max="7698" width="8.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7699" max="7699" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="7700" max="7700" width="9.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7701" max="7703" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7704" max="7704" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7705" max="7705" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7706" max="7706" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7707" max="7707" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7708" max="7943" width="11.453125" style="1"/>
-    <col min="7944" max="7944" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7945" max="7945" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7946" max="7946" width="11.453125" style="1"/>
-    <col min="7947" max="7947" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7948" max="7948" width="10.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7949" max="7949" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7950" max="7950" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7951" max="7951" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7952" max="7952" width="8.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7953" max="7953" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="7954" max="7954" width="8.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7955" max="7955" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="7956" max="7956" width="9.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7957" max="7959" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7960" max="7960" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7961" max="7961" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7962" max="7962" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7963" max="7963" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7964" max="8199" width="11.453125" style="1"/>
-    <col min="8200" max="8200" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8201" max="8201" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8202" max="8202" width="11.453125" style="1"/>
-    <col min="8203" max="8203" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8204" max="8204" width="10.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8205" max="8205" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8206" max="8206" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8207" max="8207" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8208" max="8208" width="8.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8209" max="8209" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="8210" max="8210" width="8.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8211" max="8211" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="8212" max="8212" width="9.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8213" max="8215" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8216" max="8216" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8217" max="8217" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8218" max="8218" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8219" max="8219" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8220" max="8455" width="11.453125" style="1"/>
-    <col min="8456" max="8456" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8457" max="8457" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8458" max="8458" width="11.453125" style="1"/>
-    <col min="8459" max="8459" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8460" max="8460" width="10.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8461" max="8461" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8462" max="8462" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8463" max="8463" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8464" max="8464" width="8.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8465" max="8465" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="8466" max="8466" width="8.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8467" max="8467" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="8468" max="8468" width="9.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8469" max="8471" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8472" max="8472" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8473" max="8473" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8474" max="8474" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8475" max="8475" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8476" max="8711" width="11.453125" style="1"/>
-    <col min="8712" max="8712" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8713" max="8713" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8714" max="8714" width="11.453125" style="1"/>
-    <col min="8715" max="8715" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8716" max="8716" width="10.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8717" max="8717" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8718" max="8718" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8719" max="8719" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8720" max="8720" width="8.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8721" max="8721" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="8722" max="8722" width="8.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8723" max="8723" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="8724" max="8724" width="9.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8725" max="8727" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8728" max="8728" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8729" max="8729" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8730" max="8730" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8731" max="8731" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8732" max="8967" width="11.453125" style="1"/>
-    <col min="8968" max="8968" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8969" max="8969" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8970" max="8970" width="11.453125" style="1"/>
-    <col min="8971" max="8971" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8972" max="8972" width="10.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8973" max="8973" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8974" max="8974" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8975" max="8975" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8976" max="8976" width="8.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8977" max="8977" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="8978" max="8978" width="8.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8979" max="8979" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="8980" max="8980" width="9.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8981" max="8983" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8984" max="8984" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8985" max="8985" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8986" max="8986" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8987" max="8987" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8988" max="9223" width="11.453125" style="1"/>
-    <col min="9224" max="9224" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9225" max="9225" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9226" max="9226" width="11.453125" style="1"/>
-    <col min="9227" max="9227" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9228" max="9228" width="10.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9229" max="9229" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9230" max="9230" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9231" max="9231" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9232" max="9232" width="8.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9233" max="9233" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="9234" max="9234" width="8.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9235" max="9235" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="9236" max="9236" width="9.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9237" max="9239" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9240" max="9240" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9241" max="9241" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9242" max="9242" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9243" max="9243" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9244" max="9479" width="11.453125" style="1"/>
-    <col min="9480" max="9480" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9481" max="9481" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9482" max="9482" width="11.453125" style="1"/>
-    <col min="9483" max="9483" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9484" max="9484" width="10.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9485" max="9485" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9486" max="9486" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9487" max="9487" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9488" max="9488" width="8.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9489" max="9489" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="9490" max="9490" width="8.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9491" max="9491" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="9492" max="9492" width="9.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9493" max="9495" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9496" max="9496" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9497" max="9497" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9498" max="9498" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9499" max="9499" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9500" max="9735" width="11.453125" style="1"/>
-    <col min="9736" max="9736" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9737" max="9737" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9738" max="9738" width="11.453125" style="1"/>
-    <col min="9739" max="9739" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9740" max="9740" width="10.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9741" max="9741" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9742" max="9742" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9743" max="9743" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9744" max="9744" width="8.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9745" max="9745" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="9746" max="9746" width="8.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9747" max="9747" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="9748" max="9748" width="9.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9749" max="9751" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9752" max="9752" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9753" max="9753" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9754" max="9754" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9755" max="9755" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9756" max="9991" width="11.453125" style="1"/>
-    <col min="9992" max="9992" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9993" max="9993" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9994" max="9994" width="11.453125" style="1"/>
-    <col min="9995" max="9995" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9996" max="9996" width="10.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9997" max="9997" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9998" max="9998" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9999" max="9999" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10000" max="10000" width="8.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10001" max="10001" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="10002" max="10002" width="8.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10003" max="10003" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="10004" max="10004" width="9.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10005" max="10007" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10008" max="10008" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10009" max="10009" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10010" max="10010" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10011" max="10011" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10012" max="10247" width="11.453125" style="1"/>
-    <col min="10248" max="10248" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10249" max="10249" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10250" max="10250" width="11.453125" style="1"/>
-    <col min="10251" max="10251" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10252" max="10252" width="10.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10253" max="10253" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10254" max="10254" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10255" max="10255" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10256" max="10256" width="8.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10257" max="10257" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="10258" max="10258" width="8.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10259" max="10259" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="10260" max="10260" width="9.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10261" max="10263" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10264" max="10264" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10265" max="10265" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10266" max="10266" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10267" max="10267" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10268" max="10503" width="11.453125" style="1"/>
-    <col min="10504" max="10504" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10505" max="10505" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10506" max="10506" width="11.453125" style="1"/>
-    <col min="10507" max="10507" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10508" max="10508" width="10.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10509" max="10509" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10510" max="10510" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10511" max="10511" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10512" max="10512" width="8.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10513" max="10513" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="10514" max="10514" width="8.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10515" max="10515" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="10516" max="10516" width="9.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10517" max="10519" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10520" max="10520" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10521" max="10521" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10522" max="10522" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10523" max="10523" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10524" max="10759" width="11.453125" style="1"/>
-    <col min="10760" max="10760" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10761" max="10761" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10762" max="10762" width="11.453125" style="1"/>
-    <col min="10763" max="10763" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10764" max="10764" width="10.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10765" max="10765" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10766" max="10766" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10767" max="10767" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10768" max="10768" width="8.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10769" max="10769" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="10770" max="10770" width="8.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10771" max="10771" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="10772" max="10772" width="9.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10773" max="10775" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10776" max="10776" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10777" max="10777" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10778" max="10778" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10779" max="10779" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10780" max="11015" width="11.453125" style="1"/>
-    <col min="11016" max="11016" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11017" max="11017" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11018" max="11018" width="11.453125" style="1"/>
-    <col min="11019" max="11019" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11020" max="11020" width="10.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11021" max="11021" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11022" max="11022" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11023" max="11023" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11024" max="11024" width="8.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11025" max="11025" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="11026" max="11026" width="8.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11027" max="11027" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="11028" max="11028" width="9.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11029" max="11031" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11032" max="11032" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11033" max="11033" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11034" max="11034" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11035" max="11035" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11036" max="11271" width="11.453125" style="1"/>
-    <col min="11272" max="11272" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11273" max="11273" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11274" max="11274" width="11.453125" style="1"/>
-    <col min="11275" max="11275" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11276" max="11276" width="10.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11277" max="11277" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11278" max="11278" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11279" max="11279" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11280" max="11280" width="8.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11281" max="11281" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="11282" max="11282" width="8.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11283" max="11283" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="11284" max="11284" width="9.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11285" max="11287" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11288" max="11288" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11289" max="11289" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11290" max="11290" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11291" max="11291" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11292" max="11527" width="11.453125" style="1"/>
-    <col min="11528" max="11528" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11529" max="11529" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11530" max="11530" width="11.453125" style="1"/>
-    <col min="11531" max="11531" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11532" max="11532" width="10.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11533" max="11533" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11534" max="11534" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11535" max="11535" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11536" max="11536" width="8.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11537" max="11537" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="11538" max="11538" width="8.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11539" max="11539" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="11540" max="11540" width="9.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11541" max="11543" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11544" max="11544" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11545" max="11545" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11546" max="11546" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11547" max="11547" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11548" max="11783" width="11.453125" style="1"/>
-    <col min="11784" max="11784" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11785" max="11785" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11786" max="11786" width="11.453125" style="1"/>
-    <col min="11787" max="11787" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11788" max="11788" width="10.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11789" max="11789" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11790" max="11790" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11791" max="11791" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11792" max="11792" width="8.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11793" max="11793" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="11794" max="11794" width="8.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11795" max="11795" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="11796" max="11796" width="9.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11797" max="11799" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11800" max="11800" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11801" max="11801" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11802" max="11802" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11803" max="11803" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11804" max="12039" width="11.453125" style="1"/>
-    <col min="12040" max="12040" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12041" max="12041" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12042" max="12042" width="11.453125" style="1"/>
-    <col min="12043" max="12043" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12044" max="12044" width="10.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12045" max="12045" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12046" max="12046" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12047" max="12047" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12048" max="12048" width="8.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12049" max="12049" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="12050" max="12050" width="8.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12051" max="12051" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="12052" max="12052" width="9.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12053" max="12055" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12056" max="12056" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12057" max="12057" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12058" max="12058" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12059" max="12059" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12060" max="12295" width="11.453125" style="1"/>
-    <col min="12296" max="12296" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12297" max="12297" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12298" max="12298" width="11.453125" style="1"/>
-    <col min="12299" max="12299" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12300" max="12300" width="10.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12301" max="12301" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12302" max="12302" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12303" max="12303" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12304" max="12304" width="8.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12305" max="12305" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="12306" max="12306" width="8.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12307" max="12307" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="12308" max="12308" width="9.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12309" max="12311" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12312" max="12312" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12313" max="12313" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12314" max="12314" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12315" max="12315" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12316" max="12551" width="11.453125" style="1"/>
-    <col min="12552" max="12552" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12553" max="12553" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12554" max="12554" width="11.453125" style="1"/>
-    <col min="12555" max="12555" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12556" max="12556" width="10.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12557" max="12557" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12558" max="12558" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12559" max="12559" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12560" max="12560" width="8.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12561" max="12561" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="12562" max="12562" width="8.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12563" max="12563" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="12564" max="12564" width="9.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12565" max="12567" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12568" max="12568" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12569" max="12569" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12570" max="12570" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12571" max="12571" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12572" max="12807" width="11.453125" style="1"/>
-    <col min="12808" max="12808" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12809" max="12809" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12810" max="12810" width="11.453125" style="1"/>
-    <col min="12811" max="12811" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12812" max="12812" width="10.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12813" max="12813" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12814" max="12814" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12815" max="12815" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12816" max="12816" width="8.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12817" max="12817" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="12818" max="12818" width="8.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12819" max="12819" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="12820" max="12820" width="9.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12821" max="12823" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12824" max="12824" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12825" max="12825" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12826" max="12826" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12827" max="12827" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12828" max="13063" width="11.453125" style="1"/>
-    <col min="13064" max="13064" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13065" max="13065" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13066" max="13066" width="11.453125" style="1"/>
-    <col min="13067" max="13067" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13068" max="13068" width="10.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13069" max="13069" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13070" max="13070" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13071" max="13071" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13072" max="13072" width="8.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13073" max="13073" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="13074" max="13074" width="8.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13075" max="13075" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="13076" max="13076" width="9.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13077" max="13079" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13080" max="13080" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13081" max="13081" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13082" max="13082" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13083" max="13083" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13084" max="13319" width="11.453125" style="1"/>
-    <col min="13320" max="13320" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13321" max="13321" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13322" max="13322" width="11.453125" style="1"/>
-    <col min="13323" max="13323" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13324" max="13324" width="10.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13325" max="13325" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13326" max="13326" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13327" max="13327" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13328" max="13328" width="8.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13329" max="13329" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="13330" max="13330" width="8.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13331" max="13331" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="13332" max="13332" width="9.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13333" max="13335" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13336" max="13336" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13337" max="13337" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13338" max="13338" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13339" max="13339" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13340" max="13575" width="11.453125" style="1"/>
-    <col min="13576" max="13576" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13577" max="13577" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13578" max="13578" width="11.453125" style="1"/>
-    <col min="13579" max="13579" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13580" max="13580" width="10.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13581" max="13581" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13582" max="13582" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13583" max="13583" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13584" max="13584" width="8.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13585" max="13585" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="13586" max="13586" width="8.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13587" max="13587" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="13588" max="13588" width="9.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13589" max="13591" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13592" max="13592" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13593" max="13593" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13594" max="13594" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13595" max="13595" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13596" max="13831" width="11.453125" style="1"/>
-    <col min="13832" max="13832" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13833" max="13833" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13834" max="13834" width="11.453125" style="1"/>
-    <col min="13835" max="13835" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13836" max="13836" width="10.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13837" max="13837" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13838" max="13838" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13839" max="13839" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13840" max="13840" width="8.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13841" max="13841" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="13842" max="13842" width="8.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13843" max="13843" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="13844" max="13844" width="9.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13845" max="13847" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13848" max="13848" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13849" max="13849" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13850" max="13850" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13851" max="13851" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13852" max="14087" width="11.453125" style="1"/>
-    <col min="14088" max="14088" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14089" max="14089" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="14090" max="14090" width="11.453125" style="1"/>
-    <col min="14091" max="14091" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14092" max="14092" width="10.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14093" max="14093" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14094" max="14094" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="14095" max="14095" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14096" max="14096" width="8.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14097" max="14097" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="14098" max="14098" width="8.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14099" max="14099" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="14100" max="14100" width="9.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14101" max="14103" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14104" max="14104" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14105" max="14105" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14106" max="14106" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14107" max="14107" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14108" max="14343" width="11.453125" style="1"/>
-    <col min="14344" max="14344" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14345" max="14345" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="14346" max="14346" width="11.453125" style="1"/>
-    <col min="14347" max="14347" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14348" max="14348" width="10.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14349" max="14349" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14350" max="14350" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="14351" max="14351" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14352" max="14352" width="8.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14353" max="14353" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="14354" max="14354" width="8.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14355" max="14355" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="14356" max="14356" width="9.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14357" max="14359" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14360" max="14360" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14361" max="14361" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14362" max="14362" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14363" max="14363" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14364" max="14599" width="11.453125" style="1"/>
-    <col min="14600" max="14600" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14601" max="14601" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="14602" max="14602" width="11.453125" style="1"/>
-    <col min="14603" max="14603" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14604" max="14604" width="10.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14605" max="14605" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14606" max="14606" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="14607" max="14607" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14608" max="14608" width="8.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14609" max="14609" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="14610" max="14610" width="8.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14611" max="14611" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="14612" max="14612" width="9.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14613" max="14615" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14616" max="14616" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14617" max="14617" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14618" max="14618" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14619" max="14619" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14620" max="14855" width="11.453125" style="1"/>
-    <col min="14856" max="14856" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14857" max="14857" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="14858" max="14858" width="11.453125" style="1"/>
-    <col min="14859" max="14859" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14860" max="14860" width="10.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14861" max="14861" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14862" max="14862" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="14863" max="14863" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14864" max="14864" width="8.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14865" max="14865" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="14866" max="14866" width="8.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14867" max="14867" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="14868" max="14868" width="9.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14869" max="14871" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14872" max="14872" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14873" max="14873" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14874" max="14874" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14875" max="14875" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14876" max="15111" width="11.453125" style="1"/>
-    <col min="15112" max="15112" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15113" max="15113" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="15114" max="15114" width="11.453125" style="1"/>
-    <col min="15115" max="15115" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15116" max="15116" width="10.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15117" max="15117" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15118" max="15118" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="15119" max="15119" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15120" max="15120" width="8.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15121" max="15121" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="15122" max="15122" width="8.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15123" max="15123" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="15124" max="15124" width="9.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15125" max="15127" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15128" max="15128" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15129" max="15129" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15130" max="15130" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15131" max="15131" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15132" max="15367" width="11.453125" style="1"/>
-    <col min="15368" max="15368" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15369" max="15369" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="15370" max="15370" width="11.453125" style="1"/>
-    <col min="15371" max="15371" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15372" max="15372" width="10.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15373" max="15373" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15374" max="15374" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="15375" max="15375" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15376" max="15376" width="8.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15377" max="15377" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="15378" max="15378" width="8.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15379" max="15379" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="15380" max="15380" width="9.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15381" max="15383" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15384" max="15384" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15385" max="15385" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15386" max="15386" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15387" max="15387" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15388" max="15623" width="11.453125" style="1"/>
-    <col min="15624" max="15624" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15625" max="15625" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="15626" max="15626" width="11.453125" style="1"/>
-    <col min="15627" max="15627" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15628" max="15628" width="10.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15629" max="15629" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15630" max="15630" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="15631" max="15631" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15632" max="15632" width="8.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15633" max="15633" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="15634" max="15634" width="8.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15635" max="15635" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="15636" max="15636" width="9.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15637" max="15639" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15640" max="15640" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15641" max="15641" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15642" max="15642" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15643" max="15643" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15644" max="15879" width="11.453125" style="1"/>
-    <col min="15880" max="15880" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15881" max="15881" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="15882" max="15882" width="11.453125" style="1"/>
-    <col min="15883" max="15883" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15884" max="15884" width="10.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15885" max="15885" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15886" max="15886" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="15887" max="15887" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15888" max="15888" width="8.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15889" max="15889" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="15890" max="15890" width="8.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15891" max="15891" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="15892" max="15892" width="9.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15893" max="15895" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15896" max="15896" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15897" max="15897" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15898" max="15898" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15899" max="15899" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15900" max="16135" width="11.453125" style="1"/>
-    <col min="16136" max="16136" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="16137" max="16137" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="16138" max="16138" width="11.453125" style="1"/>
-    <col min="16139" max="16139" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="16140" max="16140" width="10.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16141" max="16141" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="16142" max="16142" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="16143" max="16143" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="16144" max="16144" width="8.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16145" max="16145" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="16146" max="16146" width="8.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="16147" max="16147" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="16148" max="16148" width="9.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="16149" max="16151" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="16152" max="16152" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="16153" max="16153" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="16154" max="16154" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="16155" max="16155" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="16156" max="16384" width="11.453125" style="1"/>
+    <col min="28" max="28" width="12.08984375" style="1" customWidth="1"/>
+    <col min="29" max="29" width="12.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="264" width="11.453125" style="1"/>
+    <col min="265" max="265" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="266" max="266" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="267" max="267" width="11.453125" style="1"/>
+    <col min="268" max="268" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="269" max="269" width="10.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="270" max="270" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="271" max="271" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="272" max="272" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="273" max="273" width="8.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="274" max="274" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="275" max="275" width="8.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="276" max="276" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="277" max="277" width="9.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="278" max="280" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="281" max="281" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="282" max="282" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="283" max="283" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="284" max="284" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="285" max="520" width="11.453125" style="1"/>
+    <col min="521" max="521" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="522" max="522" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="523" max="523" width="11.453125" style="1"/>
+    <col min="524" max="524" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="525" max="525" width="10.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="526" max="526" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="527" max="527" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="528" max="528" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="529" max="529" width="8.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="530" max="530" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="531" max="531" width="8.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="532" max="532" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="533" max="533" width="9.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="534" max="536" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="537" max="537" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="538" max="538" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="539" max="539" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="540" max="540" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="541" max="776" width="11.453125" style="1"/>
+    <col min="777" max="777" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="778" max="778" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="779" max="779" width="11.453125" style="1"/>
+    <col min="780" max="780" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="781" max="781" width="10.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="782" max="782" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="783" max="783" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="784" max="784" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="785" max="785" width="8.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="786" max="786" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="787" max="787" width="8.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="788" max="788" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="789" max="789" width="9.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="790" max="792" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="793" max="793" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="794" max="794" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="795" max="795" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="796" max="796" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="797" max="1032" width="11.453125" style="1"/>
+    <col min="1033" max="1033" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1034" max="1034" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1035" max="1035" width="11.453125" style="1"/>
+    <col min="1036" max="1036" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1037" max="1037" width="10.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1038" max="1038" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1039" max="1039" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1040" max="1040" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1041" max="1041" width="8.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1042" max="1042" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="1043" max="1043" width="8.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1044" max="1044" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="1045" max="1045" width="9.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1046" max="1048" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1049" max="1049" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1050" max="1050" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1051" max="1051" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1052" max="1052" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1053" max="1288" width="11.453125" style="1"/>
+    <col min="1289" max="1289" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1290" max="1290" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1291" max="1291" width="11.453125" style="1"/>
+    <col min="1292" max="1292" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1293" max="1293" width="10.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1294" max="1294" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1295" max="1295" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1296" max="1296" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1297" max="1297" width="8.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1298" max="1298" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="1299" max="1299" width="8.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1300" max="1300" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="1301" max="1301" width="9.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1302" max="1304" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1305" max="1305" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1306" max="1306" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1307" max="1307" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1308" max="1308" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1309" max="1544" width="11.453125" style="1"/>
+    <col min="1545" max="1545" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1546" max="1546" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1547" max="1547" width="11.453125" style="1"/>
+    <col min="1548" max="1548" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1549" max="1549" width="10.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1550" max="1550" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1551" max="1551" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1552" max="1552" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1553" max="1553" width="8.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1554" max="1554" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="1555" max="1555" width="8.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1556" max="1556" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="1557" max="1557" width="9.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1558" max="1560" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1561" max="1561" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1562" max="1562" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1563" max="1563" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1564" max="1564" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1565" max="1800" width="11.453125" style="1"/>
+    <col min="1801" max="1801" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1802" max="1802" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1803" max="1803" width="11.453125" style="1"/>
+    <col min="1804" max="1804" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1805" max="1805" width="10.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1806" max="1806" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1807" max="1807" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1808" max="1808" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1809" max="1809" width="8.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1810" max="1810" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="1811" max="1811" width="8.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1812" max="1812" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="1813" max="1813" width="9.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1814" max="1816" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1817" max="1817" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1818" max="1818" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1819" max="1819" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1820" max="1820" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1821" max="2056" width="11.453125" style="1"/>
+    <col min="2057" max="2057" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2058" max="2058" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2059" max="2059" width="11.453125" style="1"/>
+    <col min="2060" max="2060" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2061" max="2061" width="10.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2062" max="2062" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2063" max="2063" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2064" max="2064" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2065" max="2065" width="8.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2066" max="2066" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="2067" max="2067" width="8.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2068" max="2068" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="2069" max="2069" width="9.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2070" max="2072" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2073" max="2073" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2074" max="2074" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2075" max="2075" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2076" max="2076" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2077" max="2312" width="11.453125" style="1"/>
+    <col min="2313" max="2313" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2314" max="2314" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2315" max="2315" width="11.453125" style="1"/>
+    <col min="2316" max="2316" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2317" max="2317" width="10.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2318" max="2318" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2319" max="2319" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2320" max="2320" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2321" max="2321" width="8.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2322" max="2322" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="2323" max="2323" width="8.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2324" max="2324" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="2325" max="2325" width="9.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2326" max="2328" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2329" max="2329" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2330" max="2330" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2331" max="2331" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2332" max="2332" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2333" max="2568" width="11.453125" style="1"/>
+    <col min="2569" max="2569" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2570" max="2570" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2571" max="2571" width="11.453125" style="1"/>
+    <col min="2572" max="2572" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2573" max="2573" width="10.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2574" max="2574" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2575" max="2575" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2576" max="2576" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2577" max="2577" width="8.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2578" max="2578" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="2579" max="2579" width="8.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2580" max="2580" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="2581" max="2581" width="9.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2582" max="2584" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2585" max="2585" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2586" max="2586" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2587" max="2587" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2588" max="2588" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2589" max="2824" width="11.453125" style="1"/>
+    <col min="2825" max="2825" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2826" max="2826" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2827" max="2827" width="11.453125" style="1"/>
+    <col min="2828" max="2828" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2829" max="2829" width="10.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2830" max="2830" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2831" max="2831" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2832" max="2832" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2833" max="2833" width="8.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2834" max="2834" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="2835" max="2835" width="8.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2836" max="2836" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="2837" max="2837" width="9.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2838" max="2840" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2841" max="2841" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2842" max="2842" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2843" max="2843" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2844" max="2844" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2845" max="3080" width="11.453125" style="1"/>
+    <col min="3081" max="3081" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3082" max="3082" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3083" max="3083" width="11.453125" style="1"/>
+    <col min="3084" max="3084" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3085" max="3085" width="10.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3086" max="3086" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3087" max="3087" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3088" max="3088" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3089" max="3089" width="8.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3090" max="3090" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="3091" max="3091" width="8.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3092" max="3092" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="3093" max="3093" width="9.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3094" max="3096" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3097" max="3097" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3098" max="3098" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3099" max="3099" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3100" max="3100" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3101" max="3336" width="11.453125" style="1"/>
+    <col min="3337" max="3337" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3338" max="3338" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3339" max="3339" width="11.453125" style="1"/>
+    <col min="3340" max="3340" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3341" max="3341" width="10.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3342" max="3342" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3343" max="3343" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3344" max="3344" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3345" max="3345" width="8.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3346" max="3346" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="3347" max="3347" width="8.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3348" max="3348" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="3349" max="3349" width="9.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3350" max="3352" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3353" max="3353" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3354" max="3354" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3355" max="3355" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3356" max="3356" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3357" max="3592" width="11.453125" style="1"/>
+    <col min="3593" max="3593" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3594" max="3594" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3595" max="3595" width="11.453125" style="1"/>
+    <col min="3596" max="3596" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3597" max="3597" width="10.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3598" max="3598" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3599" max="3599" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3600" max="3600" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3601" max="3601" width="8.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3602" max="3602" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="3603" max="3603" width="8.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3604" max="3604" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="3605" max="3605" width="9.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3606" max="3608" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3609" max="3609" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3610" max="3610" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3611" max="3611" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3612" max="3612" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3613" max="3848" width="11.453125" style="1"/>
+    <col min="3849" max="3849" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3850" max="3850" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3851" max="3851" width="11.453125" style="1"/>
+    <col min="3852" max="3852" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3853" max="3853" width="10.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3854" max="3854" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3855" max="3855" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3856" max="3856" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3857" max="3857" width="8.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3858" max="3858" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="3859" max="3859" width="8.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3860" max="3860" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="3861" max="3861" width="9.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3862" max="3864" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3865" max="3865" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3866" max="3866" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3867" max="3867" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3868" max="3868" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3869" max="4104" width="11.453125" style="1"/>
+    <col min="4105" max="4105" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4106" max="4106" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4107" max="4107" width="11.453125" style="1"/>
+    <col min="4108" max="4108" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4109" max="4109" width="10.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4110" max="4110" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4111" max="4111" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4112" max="4112" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4113" max="4113" width="8.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4114" max="4114" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="4115" max="4115" width="8.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4116" max="4116" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="4117" max="4117" width="9.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4118" max="4120" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4121" max="4121" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4122" max="4122" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4123" max="4123" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4124" max="4124" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4125" max="4360" width="11.453125" style="1"/>
+    <col min="4361" max="4361" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4362" max="4362" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4363" max="4363" width="11.453125" style="1"/>
+    <col min="4364" max="4364" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4365" max="4365" width="10.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4366" max="4366" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4367" max="4367" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4368" max="4368" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4369" max="4369" width="8.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4370" max="4370" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="4371" max="4371" width="8.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4372" max="4372" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="4373" max="4373" width="9.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4374" max="4376" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4377" max="4377" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4378" max="4378" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4379" max="4379" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4380" max="4380" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4381" max="4616" width="11.453125" style="1"/>
+    <col min="4617" max="4617" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4618" max="4618" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4619" max="4619" width="11.453125" style="1"/>
+    <col min="4620" max="4620" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4621" max="4621" width="10.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4622" max="4622" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4623" max="4623" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4624" max="4624" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4625" max="4625" width="8.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4626" max="4626" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="4627" max="4627" width="8.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4628" max="4628" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="4629" max="4629" width="9.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4630" max="4632" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4633" max="4633" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4634" max="4634" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4635" max="4635" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4636" max="4636" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4637" max="4872" width="11.453125" style="1"/>
+    <col min="4873" max="4873" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4874" max="4874" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4875" max="4875" width="11.453125" style="1"/>
+    <col min="4876" max="4876" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4877" max="4877" width="10.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4878" max="4878" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4879" max="4879" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4880" max="4880" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4881" max="4881" width="8.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4882" max="4882" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="4883" max="4883" width="8.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4884" max="4884" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="4885" max="4885" width="9.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4886" max="4888" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4889" max="4889" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4890" max="4890" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4891" max="4891" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4892" max="4892" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4893" max="5128" width="11.453125" style="1"/>
+    <col min="5129" max="5129" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5130" max="5130" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5131" max="5131" width="11.453125" style="1"/>
+    <col min="5132" max="5132" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5133" max="5133" width="10.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5134" max="5134" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5135" max="5135" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5136" max="5136" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5137" max="5137" width="8.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5138" max="5138" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="5139" max="5139" width="8.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5140" max="5140" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="5141" max="5141" width="9.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5142" max="5144" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5145" max="5145" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5146" max="5146" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5147" max="5147" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5148" max="5148" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5149" max="5384" width="11.453125" style="1"/>
+    <col min="5385" max="5385" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5386" max="5386" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5387" max="5387" width="11.453125" style="1"/>
+    <col min="5388" max="5388" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5389" max="5389" width="10.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5390" max="5390" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5391" max="5391" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5392" max="5392" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5393" max="5393" width="8.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5394" max="5394" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="5395" max="5395" width="8.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5396" max="5396" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="5397" max="5397" width="9.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5398" max="5400" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5401" max="5401" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5402" max="5402" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5403" max="5403" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5404" max="5404" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5405" max="5640" width="11.453125" style="1"/>
+    <col min="5641" max="5641" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5642" max="5642" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5643" max="5643" width="11.453125" style="1"/>
+    <col min="5644" max="5644" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5645" max="5645" width="10.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5646" max="5646" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5647" max="5647" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5648" max="5648" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5649" max="5649" width="8.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5650" max="5650" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="5651" max="5651" width="8.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5652" max="5652" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="5653" max="5653" width="9.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5654" max="5656" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5657" max="5657" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5658" max="5658" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5659" max="5659" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5660" max="5660" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5661" max="5896" width="11.453125" style="1"/>
+    <col min="5897" max="5897" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5898" max="5898" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5899" max="5899" width="11.453125" style="1"/>
+    <col min="5900" max="5900" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5901" max="5901" width="10.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5902" max="5902" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5903" max="5903" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5904" max="5904" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5905" max="5905" width="8.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5906" max="5906" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="5907" max="5907" width="8.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5908" max="5908" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="5909" max="5909" width="9.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5910" max="5912" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5913" max="5913" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5914" max="5914" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5915" max="5915" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5916" max="5916" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5917" max="6152" width="11.453125" style="1"/>
+    <col min="6153" max="6153" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6154" max="6154" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6155" max="6155" width="11.453125" style="1"/>
+    <col min="6156" max="6156" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6157" max="6157" width="10.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6158" max="6158" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6159" max="6159" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6160" max="6160" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6161" max="6161" width="8.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6162" max="6162" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="6163" max="6163" width="8.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6164" max="6164" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="6165" max="6165" width="9.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6166" max="6168" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6169" max="6169" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6170" max="6170" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6171" max="6171" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6172" max="6172" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6173" max="6408" width="11.453125" style="1"/>
+    <col min="6409" max="6409" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6410" max="6410" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6411" max="6411" width="11.453125" style="1"/>
+    <col min="6412" max="6412" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6413" max="6413" width="10.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6414" max="6414" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6415" max="6415" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6416" max="6416" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6417" max="6417" width="8.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6418" max="6418" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="6419" max="6419" width="8.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6420" max="6420" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="6421" max="6421" width="9.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6422" max="6424" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6425" max="6425" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6426" max="6426" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6427" max="6427" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6428" max="6428" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6429" max="6664" width="11.453125" style="1"/>
+    <col min="6665" max="6665" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6666" max="6666" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6667" max="6667" width="11.453125" style="1"/>
+    <col min="6668" max="6668" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6669" max="6669" width="10.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6670" max="6670" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6671" max="6671" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6672" max="6672" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6673" max="6673" width="8.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6674" max="6674" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="6675" max="6675" width="8.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6676" max="6676" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="6677" max="6677" width="9.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6678" max="6680" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6681" max="6681" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6682" max="6682" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6683" max="6683" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6684" max="6684" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6685" max="6920" width="11.453125" style="1"/>
+    <col min="6921" max="6921" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6922" max="6922" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6923" max="6923" width="11.453125" style="1"/>
+    <col min="6924" max="6924" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6925" max="6925" width="10.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6926" max="6926" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6927" max="6927" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6928" max="6928" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6929" max="6929" width="8.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6930" max="6930" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="6931" max="6931" width="8.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6932" max="6932" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="6933" max="6933" width="9.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6934" max="6936" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6937" max="6937" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6938" max="6938" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6939" max="6939" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6940" max="6940" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6941" max="7176" width="11.453125" style="1"/>
+    <col min="7177" max="7177" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7178" max="7178" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7179" max="7179" width="11.453125" style="1"/>
+    <col min="7180" max="7180" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7181" max="7181" width="10.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7182" max="7182" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7183" max="7183" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7184" max="7184" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7185" max="7185" width="8.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7186" max="7186" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="7187" max="7187" width="8.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7188" max="7188" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="7189" max="7189" width="9.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7190" max="7192" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7193" max="7193" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7194" max="7194" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7195" max="7195" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7196" max="7196" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7197" max="7432" width="11.453125" style="1"/>
+    <col min="7433" max="7433" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7434" max="7434" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7435" max="7435" width="11.453125" style="1"/>
+    <col min="7436" max="7436" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7437" max="7437" width="10.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7438" max="7438" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7439" max="7439" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7440" max="7440" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7441" max="7441" width="8.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7442" max="7442" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="7443" max="7443" width="8.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7444" max="7444" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="7445" max="7445" width="9.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7446" max="7448" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7449" max="7449" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7450" max="7450" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7451" max="7451" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7452" max="7452" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7453" max="7688" width="11.453125" style="1"/>
+    <col min="7689" max="7689" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7690" max="7690" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7691" max="7691" width="11.453125" style="1"/>
+    <col min="7692" max="7692" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7693" max="7693" width="10.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7694" max="7694" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7695" max="7695" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7696" max="7696" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7697" max="7697" width="8.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7698" max="7698" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="7699" max="7699" width="8.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7700" max="7700" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="7701" max="7701" width="9.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7702" max="7704" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7705" max="7705" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7706" max="7706" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7707" max="7707" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7708" max="7708" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7709" max="7944" width="11.453125" style="1"/>
+    <col min="7945" max="7945" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7946" max="7946" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7947" max="7947" width="11.453125" style="1"/>
+    <col min="7948" max="7948" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7949" max="7949" width="10.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7950" max="7950" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7951" max="7951" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7952" max="7952" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7953" max="7953" width="8.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7954" max="7954" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="7955" max="7955" width="8.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7956" max="7956" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="7957" max="7957" width="9.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7958" max="7960" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7961" max="7961" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7962" max="7962" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7963" max="7963" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7964" max="7964" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7965" max="8200" width="11.453125" style="1"/>
+    <col min="8201" max="8201" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8202" max="8202" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8203" max="8203" width="11.453125" style="1"/>
+    <col min="8204" max="8204" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8205" max="8205" width="10.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8206" max="8206" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8207" max="8207" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8208" max="8208" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8209" max="8209" width="8.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8210" max="8210" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="8211" max="8211" width="8.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8212" max="8212" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="8213" max="8213" width="9.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8214" max="8216" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8217" max="8217" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8218" max="8218" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8219" max="8219" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8220" max="8220" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8221" max="8456" width="11.453125" style="1"/>
+    <col min="8457" max="8457" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8458" max="8458" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8459" max="8459" width="11.453125" style="1"/>
+    <col min="8460" max="8460" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8461" max="8461" width="10.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8462" max="8462" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8463" max="8463" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8464" max="8464" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8465" max="8465" width="8.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8466" max="8466" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="8467" max="8467" width="8.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8468" max="8468" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="8469" max="8469" width="9.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8470" max="8472" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8473" max="8473" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8474" max="8474" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8475" max="8475" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8476" max="8476" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8477" max="8712" width="11.453125" style="1"/>
+    <col min="8713" max="8713" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8714" max="8714" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8715" max="8715" width="11.453125" style="1"/>
+    <col min="8716" max="8716" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8717" max="8717" width="10.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8718" max="8718" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8719" max="8719" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8720" max="8720" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8721" max="8721" width="8.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8722" max="8722" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="8723" max="8723" width="8.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8724" max="8724" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="8725" max="8725" width="9.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8726" max="8728" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8729" max="8729" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8730" max="8730" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8731" max="8731" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8732" max="8732" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8733" max="8968" width="11.453125" style="1"/>
+    <col min="8969" max="8969" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8970" max="8970" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8971" max="8971" width="11.453125" style="1"/>
+    <col min="8972" max="8972" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8973" max="8973" width="10.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8974" max="8974" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8975" max="8975" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8976" max="8976" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8977" max="8977" width="8.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8978" max="8978" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="8979" max="8979" width="8.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8980" max="8980" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="8981" max="8981" width="9.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8982" max="8984" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8985" max="8985" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8986" max="8986" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8987" max="8987" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8988" max="8988" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8989" max="9224" width="11.453125" style="1"/>
+    <col min="9225" max="9225" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9226" max="9226" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9227" max="9227" width="11.453125" style="1"/>
+    <col min="9228" max="9228" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9229" max="9229" width="10.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9230" max="9230" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9231" max="9231" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9232" max="9232" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9233" max="9233" width="8.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9234" max="9234" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="9235" max="9235" width="8.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9236" max="9236" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="9237" max="9237" width="9.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9238" max="9240" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9241" max="9241" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9242" max="9242" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9243" max="9243" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9244" max="9244" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9245" max="9480" width="11.453125" style="1"/>
+    <col min="9481" max="9481" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9482" max="9482" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9483" max="9483" width="11.453125" style="1"/>
+    <col min="9484" max="9484" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9485" max="9485" width="10.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9486" max="9486" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9487" max="9487" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9488" max="9488" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9489" max="9489" width="8.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9490" max="9490" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="9491" max="9491" width="8.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9492" max="9492" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="9493" max="9493" width="9.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9494" max="9496" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9497" max="9497" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9498" max="9498" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9499" max="9499" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9500" max="9500" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9501" max="9736" width="11.453125" style="1"/>
+    <col min="9737" max="9737" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9738" max="9738" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9739" max="9739" width="11.453125" style="1"/>
+    <col min="9740" max="9740" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9741" max="9741" width="10.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9742" max="9742" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9743" max="9743" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9744" max="9744" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9745" max="9745" width="8.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9746" max="9746" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="9747" max="9747" width="8.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9748" max="9748" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="9749" max="9749" width="9.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9750" max="9752" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9753" max="9753" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9754" max="9754" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9755" max="9755" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9756" max="9756" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9757" max="9992" width="11.453125" style="1"/>
+    <col min="9993" max="9993" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9994" max="9994" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9995" max="9995" width="11.453125" style="1"/>
+    <col min="9996" max="9996" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9997" max="9997" width="10.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9998" max="9998" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9999" max="9999" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10000" max="10000" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10001" max="10001" width="8.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10002" max="10002" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="10003" max="10003" width="8.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10004" max="10004" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="10005" max="10005" width="9.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10006" max="10008" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10009" max="10009" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10010" max="10010" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10011" max="10011" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10012" max="10012" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10013" max="10248" width="11.453125" style="1"/>
+    <col min="10249" max="10249" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10250" max="10250" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10251" max="10251" width="11.453125" style="1"/>
+    <col min="10252" max="10252" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10253" max="10253" width="10.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10254" max="10254" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10255" max="10255" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10256" max="10256" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10257" max="10257" width="8.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10258" max="10258" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="10259" max="10259" width="8.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10260" max="10260" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="10261" max="10261" width="9.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10262" max="10264" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10265" max="10265" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10266" max="10266" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10267" max="10267" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10268" max="10268" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10269" max="10504" width="11.453125" style="1"/>
+    <col min="10505" max="10505" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10506" max="10506" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10507" max="10507" width="11.453125" style="1"/>
+    <col min="10508" max="10508" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10509" max="10509" width="10.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10510" max="10510" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10511" max="10511" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10512" max="10512" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10513" max="10513" width="8.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10514" max="10514" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="10515" max="10515" width="8.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10516" max="10516" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="10517" max="10517" width="9.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10518" max="10520" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10521" max="10521" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10522" max="10522" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10523" max="10523" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10524" max="10524" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10525" max="10760" width="11.453125" style="1"/>
+    <col min="10761" max="10761" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10762" max="10762" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10763" max="10763" width="11.453125" style="1"/>
+    <col min="10764" max="10764" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10765" max="10765" width="10.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10766" max="10766" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10767" max="10767" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10768" max="10768" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10769" max="10769" width="8.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10770" max="10770" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="10771" max="10771" width="8.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10772" max="10772" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="10773" max="10773" width="9.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10774" max="10776" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10777" max="10777" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10778" max="10778" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10779" max="10779" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10780" max="10780" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10781" max="11016" width="11.453125" style="1"/>
+    <col min="11017" max="11017" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11018" max="11018" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11019" max="11019" width="11.453125" style="1"/>
+    <col min="11020" max="11020" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11021" max="11021" width="10.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11022" max="11022" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11023" max="11023" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11024" max="11024" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11025" max="11025" width="8.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11026" max="11026" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="11027" max="11027" width="8.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11028" max="11028" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="11029" max="11029" width="9.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11030" max="11032" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11033" max="11033" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11034" max="11034" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11035" max="11035" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11036" max="11036" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11037" max="11272" width="11.453125" style="1"/>
+    <col min="11273" max="11273" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11274" max="11274" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11275" max="11275" width="11.453125" style="1"/>
+    <col min="11276" max="11276" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11277" max="11277" width="10.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11278" max="11278" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11279" max="11279" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11280" max="11280" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11281" max="11281" width="8.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11282" max="11282" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="11283" max="11283" width="8.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11284" max="11284" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="11285" max="11285" width="9.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11286" max="11288" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11289" max="11289" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11290" max="11290" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11291" max="11291" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11292" max="11292" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11293" max="11528" width="11.453125" style="1"/>
+    <col min="11529" max="11529" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11530" max="11530" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11531" max="11531" width="11.453125" style="1"/>
+    <col min="11532" max="11532" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11533" max="11533" width="10.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11534" max="11534" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11535" max="11535" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11536" max="11536" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11537" max="11537" width="8.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11538" max="11538" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="11539" max="11539" width="8.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11540" max="11540" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="11541" max="11541" width="9.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11542" max="11544" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11545" max="11545" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11546" max="11546" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11547" max="11547" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11548" max="11548" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11549" max="11784" width="11.453125" style="1"/>
+    <col min="11785" max="11785" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11786" max="11786" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11787" max="11787" width="11.453125" style="1"/>
+    <col min="11788" max="11788" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11789" max="11789" width="10.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11790" max="11790" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11791" max="11791" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11792" max="11792" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11793" max="11793" width="8.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11794" max="11794" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="11795" max="11795" width="8.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11796" max="11796" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="11797" max="11797" width="9.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11798" max="11800" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11801" max="11801" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11802" max="11802" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11803" max="11803" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11804" max="11804" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11805" max="12040" width="11.453125" style="1"/>
+    <col min="12041" max="12041" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12042" max="12042" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12043" max="12043" width="11.453125" style="1"/>
+    <col min="12044" max="12044" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12045" max="12045" width="10.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12046" max="12046" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12047" max="12047" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12048" max="12048" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12049" max="12049" width="8.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12050" max="12050" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="12051" max="12051" width="8.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12052" max="12052" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="12053" max="12053" width="9.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12054" max="12056" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12057" max="12057" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12058" max="12058" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12059" max="12059" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12060" max="12060" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12061" max="12296" width="11.453125" style="1"/>
+    <col min="12297" max="12297" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12298" max="12298" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12299" max="12299" width="11.453125" style="1"/>
+    <col min="12300" max="12300" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12301" max="12301" width="10.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12302" max="12302" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12303" max="12303" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12304" max="12304" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12305" max="12305" width="8.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12306" max="12306" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="12307" max="12307" width="8.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12308" max="12308" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="12309" max="12309" width="9.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12310" max="12312" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12313" max="12313" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12314" max="12314" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12315" max="12315" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12316" max="12316" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12317" max="12552" width="11.453125" style="1"/>
+    <col min="12553" max="12553" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12554" max="12554" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12555" max="12555" width="11.453125" style="1"/>
+    <col min="12556" max="12556" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12557" max="12557" width="10.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12558" max="12558" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12559" max="12559" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12560" max="12560" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12561" max="12561" width="8.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12562" max="12562" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="12563" max="12563" width="8.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12564" max="12564" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="12565" max="12565" width="9.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12566" max="12568" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12569" max="12569" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12570" max="12570" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12571" max="12571" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12572" max="12572" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12573" max="12808" width="11.453125" style="1"/>
+    <col min="12809" max="12809" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12810" max="12810" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12811" max="12811" width="11.453125" style="1"/>
+    <col min="12812" max="12812" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12813" max="12813" width="10.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12814" max="12814" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12815" max="12815" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12816" max="12816" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12817" max="12817" width="8.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12818" max="12818" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="12819" max="12819" width="8.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12820" max="12820" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="12821" max="12821" width="9.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12822" max="12824" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12825" max="12825" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12826" max="12826" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12827" max="12827" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12828" max="12828" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12829" max="13064" width="11.453125" style="1"/>
+    <col min="13065" max="13065" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13066" max="13066" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13067" max="13067" width="11.453125" style="1"/>
+    <col min="13068" max="13068" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13069" max="13069" width="10.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13070" max="13070" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13071" max="13071" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13072" max="13072" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13073" max="13073" width="8.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13074" max="13074" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="13075" max="13075" width="8.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13076" max="13076" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="13077" max="13077" width="9.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13078" max="13080" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13081" max="13081" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13082" max="13082" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13083" max="13083" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13084" max="13084" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13085" max="13320" width="11.453125" style="1"/>
+    <col min="13321" max="13321" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13322" max="13322" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13323" max="13323" width="11.453125" style="1"/>
+    <col min="13324" max="13324" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13325" max="13325" width="10.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13326" max="13326" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13327" max="13327" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13328" max="13328" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13329" max="13329" width="8.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13330" max="13330" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="13331" max="13331" width="8.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13332" max="13332" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="13333" max="13333" width="9.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13334" max="13336" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13337" max="13337" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13338" max="13338" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13339" max="13339" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13340" max="13340" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13341" max="13576" width="11.453125" style="1"/>
+    <col min="13577" max="13577" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13578" max="13578" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13579" max="13579" width="11.453125" style="1"/>
+    <col min="13580" max="13580" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13581" max="13581" width="10.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13582" max="13582" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13583" max="13583" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13584" max="13584" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13585" max="13585" width="8.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13586" max="13586" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="13587" max="13587" width="8.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13588" max="13588" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="13589" max="13589" width="9.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13590" max="13592" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13593" max="13593" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13594" max="13594" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13595" max="13595" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13596" max="13596" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13597" max="13832" width="11.453125" style="1"/>
+    <col min="13833" max="13833" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13834" max="13834" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13835" max="13835" width="11.453125" style="1"/>
+    <col min="13836" max="13836" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13837" max="13837" width="10.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13838" max="13838" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13839" max="13839" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13840" max="13840" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13841" max="13841" width="8.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13842" max="13842" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="13843" max="13843" width="8.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13844" max="13844" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="13845" max="13845" width="9.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13846" max="13848" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13849" max="13849" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13850" max="13850" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13851" max="13851" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13852" max="13852" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13853" max="14088" width="11.453125" style="1"/>
+    <col min="14089" max="14089" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14090" max="14090" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14091" max="14091" width="11.453125" style="1"/>
+    <col min="14092" max="14092" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14093" max="14093" width="10.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14094" max="14094" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14095" max="14095" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14096" max="14096" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14097" max="14097" width="8.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14098" max="14098" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="14099" max="14099" width="8.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14100" max="14100" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="14101" max="14101" width="9.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14102" max="14104" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14105" max="14105" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14106" max="14106" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14107" max="14107" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14108" max="14108" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14109" max="14344" width="11.453125" style="1"/>
+    <col min="14345" max="14345" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14346" max="14346" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14347" max="14347" width="11.453125" style="1"/>
+    <col min="14348" max="14348" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14349" max="14349" width="10.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14350" max="14350" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14351" max="14351" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14352" max="14352" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14353" max="14353" width="8.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14354" max="14354" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="14355" max="14355" width="8.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14356" max="14356" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="14357" max="14357" width="9.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14358" max="14360" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14361" max="14361" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14362" max="14362" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14363" max="14363" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14364" max="14364" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14365" max="14600" width="11.453125" style="1"/>
+    <col min="14601" max="14601" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14602" max="14602" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14603" max="14603" width="11.453125" style="1"/>
+    <col min="14604" max="14604" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14605" max="14605" width="10.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14606" max="14606" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14607" max="14607" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14608" max="14608" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14609" max="14609" width="8.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14610" max="14610" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="14611" max="14611" width="8.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14612" max="14612" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="14613" max="14613" width="9.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14614" max="14616" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14617" max="14617" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14618" max="14618" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14619" max="14619" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14620" max="14620" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14621" max="14856" width="11.453125" style="1"/>
+    <col min="14857" max="14857" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14858" max="14858" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14859" max="14859" width="11.453125" style="1"/>
+    <col min="14860" max="14860" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14861" max="14861" width="10.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14862" max="14862" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14863" max="14863" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14864" max="14864" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14865" max="14865" width="8.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14866" max="14866" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="14867" max="14867" width="8.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14868" max="14868" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="14869" max="14869" width="9.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14870" max="14872" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14873" max="14873" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14874" max="14874" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14875" max="14875" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14876" max="14876" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14877" max="15112" width="11.453125" style="1"/>
+    <col min="15113" max="15113" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15114" max="15114" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15115" max="15115" width="11.453125" style="1"/>
+    <col min="15116" max="15116" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15117" max="15117" width="10.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15118" max="15118" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15119" max="15119" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15120" max="15120" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15121" max="15121" width="8.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15122" max="15122" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="15123" max="15123" width="8.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15124" max="15124" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="15125" max="15125" width="9.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15126" max="15128" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15129" max="15129" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15130" max="15130" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15131" max="15131" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15132" max="15132" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15133" max="15368" width="11.453125" style="1"/>
+    <col min="15369" max="15369" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15370" max="15370" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15371" max="15371" width="11.453125" style="1"/>
+    <col min="15372" max="15372" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15373" max="15373" width="10.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15374" max="15374" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15375" max="15375" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15376" max="15376" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15377" max="15377" width="8.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15378" max="15378" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="15379" max="15379" width="8.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15380" max="15380" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="15381" max="15381" width="9.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15382" max="15384" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15385" max="15385" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15386" max="15386" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15387" max="15387" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15388" max="15388" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15389" max="15624" width="11.453125" style="1"/>
+    <col min="15625" max="15625" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15626" max="15626" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15627" max="15627" width="11.453125" style="1"/>
+    <col min="15628" max="15628" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15629" max="15629" width="10.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15630" max="15630" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15631" max="15631" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15632" max="15632" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15633" max="15633" width="8.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15634" max="15634" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="15635" max="15635" width="8.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15636" max="15636" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="15637" max="15637" width="9.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15638" max="15640" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15641" max="15641" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15642" max="15642" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15643" max="15643" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15644" max="15644" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15645" max="15880" width="11.453125" style="1"/>
+    <col min="15881" max="15881" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15882" max="15882" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15883" max="15883" width="11.453125" style="1"/>
+    <col min="15884" max="15884" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15885" max="15885" width="10.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15886" max="15886" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15887" max="15887" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15888" max="15888" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15889" max="15889" width="8.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15890" max="15890" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="15891" max="15891" width="8.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15892" max="15892" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="15893" max="15893" width="9.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15894" max="15896" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15897" max="15897" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15898" max="15898" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15899" max="15899" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15900" max="15900" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15901" max="16136" width="11.453125" style="1"/>
+    <col min="16137" max="16137" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16138" max="16138" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="16139" max="16139" width="11.453125" style="1"/>
+    <col min="16140" max="16140" width="11.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16141" max="16141" width="10.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16142" max="16142" width="13.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="16143" max="16143" width="12.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="16144" max="16144" width="8.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="16145" max="16145" width="8.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16146" max="16146" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="16147" max="16147" width="8.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16148" max="16148" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="16149" max="16149" width="9.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16150" max="16152" width="10.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16153" max="16153" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="16154" max="16154" width="9.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16155" max="16155" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="16156" max="16156" width="16.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="16157" max="16384" width="11.453125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>51</v>
       </c>
@@ -2147,10 +2161,13 @@
         <v>53</v>
       </c>
       <c r="AB1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AC1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -2203,10 +2220,13 @@
         <v>864.6</v>
       </c>
       <c r="AB2" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC2" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
@@ -2259,10 +2279,13 @@
         <v>1044</v>
       </c>
       <c r="AB3" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC3" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>32</v>
       </c>
@@ -2330,10 +2353,13 @@
         <v>146.1</v>
       </c>
       <c r="AB4" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC4" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>32</v>
       </c>
@@ -2401,10 +2427,13 @@
         <v>207.6</v>
       </c>
       <c r="AB5" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC5" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>32</v>
       </c>
@@ -2472,10 +2501,13 @@
         <v>273.89999999999998</v>
       </c>
       <c r="AB6" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC6" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>32</v>
       </c>
@@ -2543,10 +2575,13 @@
         <v>344.3</v>
       </c>
       <c r="AB7" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC7" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>32</v>
       </c>
@@ -2614,10 +2649,13 @@
         <v>493.3</v>
       </c>
       <c r="AB8" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC8" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>32</v>
       </c>
@@ -2685,10 +2723,13 @@
         <v>483.2</v>
       </c>
       <c r="AB9" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC9" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>32</v>
       </c>
@@ -2756,10 +2797,13 @@
         <v>58.5</v>
       </c>
       <c r="AB10" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC10" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>32</v>
       </c>
@@ -2827,10 +2871,13 @@
         <v>146.1</v>
       </c>
       <c r="AB11" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC11" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>32</v>
       </c>
@@ -2898,10 +2945,13 @@
         <v>273.89999999999998</v>
       </c>
       <c r="AB12" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC12" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>32</v>
       </c>
@@ -2969,10 +3019,13 @@
         <v>165.5</v>
       </c>
       <c r="AB13" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC13" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>32</v>
       </c>
@@ -3040,10 +3093,13 @@
         <v>310.2</v>
       </c>
       <c r="AB14" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC14" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>32</v>
       </c>
@@ -3111,10 +3167,13 @@
         <v>175.5</v>
       </c>
       <c r="AB15" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC15" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>32</v>
       </c>
@@ -3182,10 +3241,13 @@
         <v>328.7</v>
       </c>
       <c r="AB16" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC16" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>32</v>
       </c>
@@ -3253,10 +3315,13 @@
         <v>591.70000000000005</v>
       </c>
       <c r="AB17" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC17" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>32</v>
       </c>
@@ -3324,10 +3389,13 @@
         <v>175.5</v>
       </c>
       <c r="AB18" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC18" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>32</v>
       </c>
@@ -3395,10 +3463,13 @@
         <v>328.7</v>
       </c>
       <c r="AB19" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC19" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>32</v>
       </c>
@@ -3466,10 +3537,13 @@
         <v>141.5</v>
       </c>
       <c r="AB20" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC20" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>32</v>
       </c>
@@ -3537,10 +3611,13 @@
         <v>189.9</v>
       </c>
       <c r="AB21" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC21" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>32</v>
       </c>
@@ -3608,10 +3685,13 @@
         <v>356</v>
       </c>
       <c r="AB22" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC22" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>32</v>
       </c>
@@ -3679,10 +3759,13 @@
         <v>204.8</v>
       </c>
       <c r="AB23" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC23" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>44</v>
       </c>
@@ -3749,14 +3832,14 @@
       <c r="Y24" s="1">
         <v>207.6</v>
       </c>
-      <c r="AA24" s="1" t="s">
-        <v>75</v>
-      </c>
       <c r="AB24" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC24" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>44</v>
       </c>
@@ -3824,81 +3907,87 @@
         <v>273.89999999999998</v>
       </c>
       <c r="AB25" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC25" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+    <row r="26" spans="1:29" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C26" s="1">
+      <c r="C26" s="5">
         <v>795</v>
       </c>
-      <c r="D26" s="1">
+      <c r="D26" s="5">
         <v>26</v>
       </c>
-      <c r="E26" s="1">
+      <c r="E26" s="5">
         <v>7</v>
       </c>
-      <c r="F26" s="1">
+      <c r="F26" s="5">
         <v>0.1749</v>
       </c>
-      <c r="G26" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="H26" s="1">
+      <c r="G26" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="H26" s="5">
         <v>0.13600000000000001</v>
       </c>
-      <c r="I26" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="J26" s="1">
+      <c r="I26" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="J26" s="5">
         <v>0.40799999999999997</v>
       </c>
-      <c r="K26" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="L26" s="1">
+      <c r="K26" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="L26" s="5">
         <v>1.1080000000000001</v>
       </c>
-      <c r="M26" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q26" s="1">
+      <c r="M26" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q26" s="5">
         <v>25</v>
       </c>
-      <c r="R26" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="S26" s="1">
-        <v>75</v>
-      </c>
-      <c r="T26" s="1">
+      <c r="R26" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="S26" s="5">
+        <v>75</v>
+      </c>
+      <c r="T26" s="5">
         <v>0.1135</v>
       </c>
-      <c r="U26" s="1">
+      <c r="U26" s="5">
         <v>0.13589999999999999</v>
       </c>
-      <c r="V26" s="1">
+      <c r="V26" s="5">
         <v>5280</v>
       </c>
-      <c r="W26" s="1" t="s">
+      <c r="W26" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="X26" s="1">
+      <c r="X26" s="5">
         <v>749.1</v>
       </c>
-      <c r="Y26" s="1">
+      <c r="Y26" s="5">
         <v>344.3</v>
       </c>
-      <c r="AB26" s="1" t="s">
+      <c r="AB26" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC26" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>44</v>
       </c>
@@ -3966,10 +4055,13 @@
         <v>483.2</v>
       </c>
       <c r="AB27" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC27" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>44</v>
       </c>
@@ -4037,10 +4129,13 @@
         <v>108.6</v>
       </c>
       <c r="AB28" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC28" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>44</v>
       </c>
@@ -4108,10 +4203,13 @@
         <v>146.1</v>
       </c>
       <c r="AB29" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC29" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>44</v>
       </c>
@@ -4179,10 +4277,13 @@
         <v>273.89999999999998</v>
       </c>
       <c r="AB30" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC30" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>49</v>
       </c>
@@ -4229,10 +4330,13 @@
         <v>1544</v>
       </c>
       <c r="AB31" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC31" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>49</v>
       </c>
@@ -4279,56 +4383,15 @@
         <v>3088</v>
       </c>
       <c r="AB32" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC32" s="1" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C33" s="1">
-        <v>555</v>
-      </c>
-      <c r="D33" s="1">
-        <v>55</v>
-      </c>
-      <c r="E33" s="1">
-        <v>4</v>
-      </c>
-      <c r="F33" s="1">
-        <v>0.16439999999999999</v>
-      </c>
-      <c r="L33" s="1">
-        <v>1.1508</v>
-      </c>
-      <c r="Q33" s="1">
-        <v>25</v>
-      </c>
-      <c r="R33" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="S33" s="1">
-        <v>75</v>
-      </c>
-      <c r="T33" s="1">
-        <v>6.4000000000000001E-2</v>
-      </c>
-      <c r="U33" s="1">
-        <v>7.4399999999999994E-2</v>
-      </c>
-      <c r="V33" s="1">
-        <v>5280</v>
-      </c>
-      <c r="W33" s="1" t="s">
-        <v>55</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:WWI32" xr:uid="{37CC4BCD-4400-4E7C-96DC-CDFA2CE28B1F}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AB32">
+  <autoFilter ref="A1:WWJ32" xr:uid="{37CC4BCD-4400-4E7C-96DC-CDFA2CE28B1F}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AC32">
     <sortCondition ref="A2:A32"/>
     <sortCondition ref="C2:C32"/>
     <sortCondition ref="D2:D32"/>

</xml_diff>